<commit_message>
partial importing products, need to create import screen
</commit_message>
<xml_diff>
--- a/source-data/products/products-list.xlsx
+++ b/source-data/products/products-list.xlsx
@@ -1,10 +1,10 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="9303"/>
-  <workbookPr defaultThemeVersion="124226"/>
+  <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="27526"/>
+  <workbookPr autoCompressPictures="0"/>
   <bookViews>
-    <workbookView xWindow="120" yWindow="90" windowWidth="20115" windowHeight="7755"/>
+    <workbookView xWindow="120" yWindow="100" windowWidth="30060" windowHeight="15400"/>
   </bookViews>
   <sheets>
     <sheet name="Plan1" sheetId="1" r:id="rId1"/>
@@ -14,7 +14,12 @@
   <definedNames>
     <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">Plan1!$A$1:$D$128</definedName>
   </definedNames>
-  <calcPr calcId="145621"/>
+  <calcPr calcId="140001" concurrentCalc="0"/>
+  <extLst>
+    <ext xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" uri="{7523E5D3-25F3-A5E0-1632-64F254C22452}">
+      <mx:ArchID Flags="2"/>
+    </ext>
+  </extLst>
 </workbook>
 </file>
 
@@ -420,9 +425,6 @@
     <t>Unidade</t>
   </si>
   <si>
-    <t>Prioridade do Item</t>
-  </si>
-  <si>
     <t>Unidade(s)</t>
   </si>
   <si>
@@ -448,6 +450,9 @@
   </si>
   <si>
     <t>Recomendamos que apenas os itens marcados como prioritários fiquem listados para o usuário selecionar as quantidades. Pode haver uma lista suspensa em um campo "Outros" para ele selecionar os demais itens. Pois o foco deve ser nos itens prioritários.</t>
+  </si>
+  <si>
+    <t>Prioridade</t>
   </si>
 </sst>
 </file>
@@ -820,19 +825,19 @@
   <dimension ref="A1:H129"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="B1" workbookViewId="0">
-      <selection activeCell="H7" sqref="H7"/>
+      <selection activeCell="H21" sqref="H21"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="14" x14ac:dyDescent="0"/>
   <cols>
-    <col min="1" max="1" width="56.140625" customWidth="1"/>
-    <col min="2" max="2" width="15.42578125" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="15.7109375" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="17.85546875" bestFit="1" customWidth="1"/>
-    <col min="8" max="8" width="77.5703125" customWidth="1"/>
+    <col min="1" max="1" width="56.1640625" customWidth="1"/>
+    <col min="2" max="2" width="15.5" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="15.6640625" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="17.83203125" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="77.5" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:8">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -843,10 +848,10 @@
         <v>132</v>
       </c>
       <c r="D1" s="1" t="s">
-        <v>133</v>
-      </c>
-    </row>
-    <row r="2" spans="1:8" x14ac:dyDescent="0.25">
+        <v>142</v>
+      </c>
+    </row>
+    <row r="2" spans="1:8">
       <c r="A2" t="s">
         <v>123</v>
       </c>
@@ -854,16 +859,16 @@
         <v>3</v>
       </c>
       <c r="C2" t="s">
-        <v>134</v>
+        <v>133</v>
       </c>
       <c r="D2" t="s">
-        <v>136</v>
+        <v>135</v>
       </c>
       <c r="H2" s="3" t="s">
-        <v>140</v>
-      </c>
-    </row>
-    <row r="3" spans="1:8" ht="45" x14ac:dyDescent="0.25">
+        <v>139</v>
+      </c>
+    </row>
+    <row r="3" spans="1:8" ht="42">
       <c r="A3" t="s">
         <v>80</v>
       </c>
@@ -871,16 +876,16 @@
         <v>3</v>
       </c>
       <c r="C3" t="s">
-        <v>134</v>
+        <v>133</v>
       </c>
       <c r="D3" t="s">
-        <v>136</v>
+        <v>135</v>
       </c>
       <c r="H3" s="2" t="s">
-        <v>141</v>
-      </c>
-    </row>
-    <row r="4" spans="1:8" x14ac:dyDescent="0.25">
+        <v>140</v>
+      </c>
+    </row>
+    <row r="4" spans="1:8">
       <c r="A4" t="s">
         <v>42</v>
       </c>
@@ -888,16 +893,16 @@
         <v>3</v>
       </c>
       <c r="C4" t="s">
-        <v>139</v>
+        <v>138</v>
       </c>
       <c r="D4" t="s">
-        <v>135</v>
+        <v>134</v>
       </c>
       <c r="H4" s="4" t="s">
-        <v>134</v>
-      </c>
-    </row>
-    <row r="5" spans="1:8" x14ac:dyDescent="0.25">
+        <v>133</v>
+      </c>
+    </row>
+    <row r="5" spans="1:8">
       <c r="A5" t="s">
         <v>34</v>
       </c>
@@ -905,16 +910,16 @@
         <v>3</v>
       </c>
       <c r="C5" t="s">
-        <v>134</v>
+        <v>133</v>
       </c>
       <c r="D5" t="s">
-        <v>136</v>
+        <v>135</v>
       </c>
       <c r="H5" s="4" t="s">
-        <v>139</v>
-      </c>
-    </row>
-    <row r="6" spans="1:8" ht="47.25" customHeight="1" x14ac:dyDescent="0.25">
+        <v>138</v>
+      </c>
+    </row>
+    <row r="6" spans="1:8" ht="47.25" customHeight="1">
       <c r="A6" t="s">
         <v>31</v>
       </c>
@@ -922,16 +927,16 @@
         <v>3</v>
       </c>
       <c r="C6" t="s">
-        <v>139</v>
+        <v>138</v>
       </c>
       <c r="D6" t="s">
-        <v>135</v>
+        <v>134</v>
       </c>
       <c r="H6" s="2" t="s">
-        <v>142</v>
-      </c>
-    </row>
-    <row r="7" spans="1:8" x14ac:dyDescent="0.25">
+        <v>141</v>
+      </c>
+    </row>
+    <row r="7" spans="1:8">
       <c r="A7" t="s">
         <v>71</v>
       </c>
@@ -939,13 +944,13 @@
         <v>18</v>
       </c>
       <c r="C7" t="s">
-        <v>134</v>
+        <v>133</v>
       </c>
       <c r="D7" t="s">
-        <v>136</v>
-      </c>
-    </row>
-    <row r="8" spans="1:8" x14ac:dyDescent="0.25">
+        <v>135</v>
+      </c>
+    </row>
+    <row r="8" spans="1:8">
       <c r="A8" t="s">
         <v>102</v>
       </c>
@@ -953,13 +958,13 @@
         <v>3</v>
       </c>
       <c r="C8" t="s">
-        <v>134</v>
+        <v>133</v>
       </c>
       <c r="D8" t="s">
-        <v>136</v>
-      </c>
-    </row>
-    <row r="9" spans="1:8" x14ac:dyDescent="0.25">
+        <v>135</v>
+      </c>
+    </row>
+    <row r="9" spans="1:8">
       <c r="A9" t="s">
         <v>58</v>
       </c>
@@ -967,13 +972,13 @@
         <v>18</v>
       </c>
       <c r="C9" t="s">
-        <v>134</v>
+        <v>133</v>
       </c>
       <c r="D9" t="s">
-        <v>136</v>
-      </c>
-    </row>
-    <row r="10" spans="1:8" x14ac:dyDescent="0.25">
+        <v>135</v>
+      </c>
+    </row>
+    <row r="10" spans="1:8">
       <c r="A10" t="s">
         <v>93</v>
       </c>
@@ -981,13 +986,13 @@
         <v>3</v>
       </c>
       <c r="C10" t="s">
-        <v>134</v>
+        <v>133</v>
       </c>
       <c r="D10" t="s">
-        <v>136</v>
-      </c>
-    </row>
-    <row r="11" spans="1:8" x14ac:dyDescent="0.25">
+        <v>135</v>
+      </c>
+    </row>
+    <row r="11" spans="1:8">
       <c r="A11" t="s">
         <v>14</v>
       </c>
@@ -995,13 +1000,13 @@
         <v>3</v>
       </c>
       <c r="C11" t="s">
+        <v>133</v>
+      </c>
+      <c r="D11" t="s">
         <v>134</v>
       </c>
-      <c r="D11" t="s">
-        <v>135</v>
-      </c>
-    </row>
-    <row r="12" spans="1:8" x14ac:dyDescent="0.25">
+    </row>
+    <row r="12" spans="1:8">
       <c r="A12" t="s">
         <v>118</v>
       </c>
@@ -1009,13 +1014,13 @@
         <v>18</v>
       </c>
       <c r="C12" t="s">
-        <v>134</v>
+        <v>133</v>
       </c>
       <c r="D12" t="s">
-        <v>136</v>
-      </c>
-    </row>
-    <row r="13" spans="1:8" x14ac:dyDescent="0.25">
+        <v>135</v>
+      </c>
+    </row>
+    <row r="13" spans="1:8">
       <c r="A13" t="s">
         <v>117</v>
       </c>
@@ -1023,13 +1028,13 @@
         <v>18</v>
       </c>
       <c r="C13" t="s">
-        <v>134</v>
+        <v>133</v>
       </c>
       <c r="D13" t="s">
-        <v>136</v>
-      </c>
-    </row>
-    <row r="14" spans="1:8" x14ac:dyDescent="0.25">
+        <v>135</v>
+      </c>
+    </row>
+    <row r="14" spans="1:8">
       <c r="A14" t="s">
         <v>15</v>
       </c>
@@ -1037,13 +1042,13 @@
         <v>3</v>
       </c>
       <c r="C14" t="s">
-        <v>134</v>
+        <v>133</v>
       </c>
       <c r="D14" t="s">
-        <v>136</v>
-      </c>
-    </row>
-    <row r="15" spans="1:8" x14ac:dyDescent="0.25">
+        <v>135</v>
+      </c>
+    </row>
+    <row r="15" spans="1:8">
       <c r="A15" t="s">
         <v>55</v>
       </c>
@@ -1051,13 +1056,13 @@
         <v>3</v>
       </c>
       <c r="C15" t="s">
-        <v>134</v>
+        <v>133</v>
       </c>
       <c r="D15" t="s">
-        <v>136</v>
-      </c>
-    </row>
-    <row r="16" spans="1:8" x14ac:dyDescent="0.25">
+        <v>135</v>
+      </c>
+    </row>
+    <row r="16" spans="1:8">
       <c r="A16" t="s">
         <v>94</v>
       </c>
@@ -1065,13 +1070,13 @@
         <v>18</v>
       </c>
       <c r="C16" t="s">
-        <v>134</v>
+        <v>133</v>
       </c>
       <c r="D16" t="s">
-        <v>136</v>
-      </c>
-    </row>
-    <row r="17" spans="1:4" x14ac:dyDescent="0.25">
+        <v>135</v>
+      </c>
+    </row>
+    <row r="17" spans="1:4">
       <c r="A17" t="s">
         <v>59</v>
       </c>
@@ -1079,13 +1084,13 @@
         <v>18</v>
       </c>
       <c r="C17" t="s">
-        <v>134</v>
+        <v>133</v>
       </c>
       <c r="D17" t="s">
-        <v>136</v>
-      </c>
-    </row>
-    <row r="18" spans="1:4" x14ac:dyDescent="0.25">
+        <v>135</v>
+      </c>
+    </row>
+    <row r="18" spans="1:4">
       <c r="A18" t="s">
         <v>29</v>
       </c>
@@ -1093,13 +1098,13 @@
         <v>18</v>
       </c>
       <c r="C18" t="s">
-        <v>134</v>
+        <v>133</v>
       </c>
       <c r="D18" t="s">
-        <v>136</v>
-      </c>
-    </row>
-    <row r="19" spans="1:4" x14ac:dyDescent="0.25">
+        <v>135</v>
+      </c>
+    </row>
+    <row r="19" spans="1:4">
       <c r="A19" t="s">
         <v>124</v>
       </c>
@@ -1107,13 +1112,13 @@
         <v>18</v>
       </c>
       <c r="C19" t="s">
-        <v>134</v>
+        <v>133</v>
       </c>
       <c r="D19" t="s">
-        <v>136</v>
-      </c>
-    </row>
-    <row r="20" spans="1:4" x14ac:dyDescent="0.25">
+        <v>135</v>
+      </c>
+    </row>
+    <row r="20" spans="1:4">
       <c r="A20" t="s">
         <v>60</v>
       </c>
@@ -1121,13 +1126,13 @@
         <v>18</v>
       </c>
       <c r="C20" t="s">
-        <v>134</v>
+        <v>133</v>
       </c>
       <c r="D20" t="s">
-        <v>136</v>
-      </c>
-    </row>
-    <row r="21" spans="1:4" x14ac:dyDescent="0.25">
+        <v>135</v>
+      </c>
+    </row>
+    <row r="21" spans="1:4">
       <c r="A21" t="s">
         <v>43</v>
       </c>
@@ -1135,13 +1140,13 @@
         <v>18</v>
       </c>
       <c r="C21" t="s">
-        <v>134</v>
+        <v>133</v>
       </c>
       <c r="D21" t="s">
-        <v>136</v>
-      </c>
-    </row>
-    <row r="22" spans="1:4" x14ac:dyDescent="0.25">
+        <v>135</v>
+      </c>
+    </row>
+    <row r="22" spans="1:4">
       <c r="A22" t="s">
         <v>120</v>
       </c>
@@ -1149,13 +1154,13 @@
         <v>3</v>
       </c>
       <c r="C22" t="s">
-        <v>134</v>
+        <v>133</v>
       </c>
       <c r="D22" t="s">
-        <v>136</v>
-      </c>
-    </row>
-    <row r="23" spans="1:4" x14ac:dyDescent="0.25">
+        <v>135</v>
+      </c>
+    </row>
+    <row r="23" spans="1:4">
       <c r="A23" t="s">
         <v>81</v>
       </c>
@@ -1163,13 +1168,13 @@
         <v>3</v>
       </c>
       <c r="C23" t="s">
-        <v>134</v>
+        <v>133</v>
       </c>
       <c r="D23" t="s">
-        <v>136</v>
-      </c>
-    </row>
-    <row r="24" spans="1:4" x14ac:dyDescent="0.25">
+        <v>135</v>
+      </c>
+    </row>
+    <row r="24" spans="1:4">
       <c r="A24" t="s">
         <v>82</v>
       </c>
@@ -1177,13 +1182,13 @@
         <v>3</v>
       </c>
       <c r="C24" t="s">
-        <v>134</v>
+        <v>133</v>
       </c>
       <c r="D24" t="s">
-        <v>136</v>
-      </c>
-    </row>
-    <row r="25" spans="1:4" x14ac:dyDescent="0.25">
+        <v>135</v>
+      </c>
+    </row>
+    <row r="25" spans="1:4">
       <c r="A25" t="s">
         <v>22</v>
       </c>
@@ -1191,13 +1196,13 @@
         <v>3</v>
       </c>
       <c r="C25" t="s">
-        <v>134</v>
+        <v>133</v>
       </c>
       <c r="D25" t="s">
-        <v>136</v>
-      </c>
-    </row>
-    <row r="26" spans="1:4" x14ac:dyDescent="0.25">
+        <v>135</v>
+      </c>
+    </row>
+    <row r="26" spans="1:4">
       <c r="A26" t="s">
         <v>27</v>
       </c>
@@ -1205,13 +1210,13 @@
         <v>18</v>
       </c>
       <c r="C26" t="s">
-        <v>134</v>
+        <v>133</v>
       </c>
       <c r="D26" t="s">
-        <v>136</v>
-      </c>
-    </row>
-    <row r="27" spans="1:4" x14ac:dyDescent="0.25">
+        <v>135</v>
+      </c>
+    </row>
+    <row r="27" spans="1:4">
       <c r="A27" t="s">
         <v>33</v>
       </c>
@@ -1219,13 +1224,13 @@
         <v>18</v>
       </c>
       <c r="C27" t="s">
-        <v>134</v>
+        <v>133</v>
       </c>
       <c r="D27" t="s">
-        <v>136</v>
-      </c>
-    </row>
-    <row r="28" spans="1:4" x14ac:dyDescent="0.25">
+        <v>135</v>
+      </c>
+    </row>
+    <row r="28" spans="1:4">
       <c r="A28" t="s">
         <v>95</v>
       </c>
@@ -1233,13 +1238,13 @@
         <v>3</v>
       </c>
       <c r="C28" t="s">
-        <v>134</v>
+        <v>133</v>
       </c>
       <c r="D28" t="s">
-        <v>136</v>
-      </c>
-    </row>
-    <row r="29" spans="1:4" x14ac:dyDescent="0.25">
+        <v>135</v>
+      </c>
+    </row>
+    <row r="29" spans="1:4">
       <c r="A29" t="s">
         <v>103</v>
       </c>
@@ -1247,13 +1252,13 @@
         <v>18</v>
       </c>
       <c r="C29" t="s">
-        <v>134</v>
+        <v>133</v>
       </c>
       <c r="D29" t="s">
-        <v>136</v>
-      </c>
-    </row>
-    <row r="30" spans="1:4" x14ac:dyDescent="0.25">
+        <v>135</v>
+      </c>
+    </row>
+    <row r="30" spans="1:4">
       <c r="A30" t="s">
         <v>78</v>
       </c>
@@ -1261,13 +1266,13 @@
         <v>18</v>
       </c>
       <c r="C30" t="s">
-        <v>134</v>
+        <v>133</v>
       </c>
       <c r="D30" t="s">
-        <v>136</v>
-      </c>
-    </row>
-    <row r="31" spans="1:4" x14ac:dyDescent="0.25">
+        <v>135</v>
+      </c>
+    </row>
+    <row r="31" spans="1:4">
       <c r="A31" t="s">
         <v>83</v>
       </c>
@@ -1275,13 +1280,13 @@
         <v>3</v>
       </c>
       <c r="C31" t="s">
-        <v>134</v>
+        <v>133</v>
       </c>
       <c r="D31" t="s">
-        <v>136</v>
-      </c>
-    </row>
-    <row r="32" spans="1:4" x14ac:dyDescent="0.25">
+        <v>135</v>
+      </c>
+    </row>
+    <row r="32" spans="1:4">
       <c r="A32" t="s">
         <v>84</v>
       </c>
@@ -1289,13 +1294,13 @@
         <v>3</v>
       </c>
       <c r="C32" t="s">
-        <v>134</v>
+        <v>133</v>
       </c>
       <c r="D32" t="s">
-        <v>136</v>
-      </c>
-    </row>
-    <row r="33" spans="1:4" x14ac:dyDescent="0.25">
+        <v>135</v>
+      </c>
+    </row>
+    <row r="33" spans="1:4">
       <c r="A33" t="s">
         <v>35</v>
       </c>
@@ -1303,13 +1308,13 @@
         <v>18</v>
       </c>
       <c r="C33" t="s">
-        <v>134</v>
+        <v>133</v>
       </c>
       <c r="D33" t="s">
-        <v>136</v>
-      </c>
-    </row>
-    <row r="34" spans="1:4" x14ac:dyDescent="0.25">
+        <v>135</v>
+      </c>
+    </row>
+    <row r="34" spans="1:4">
       <c r="A34" t="s">
         <v>36</v>
       </c>
@@ -1317,13 +1322,13 @@
         <v>3</v>
       </c>
       <c r="C34" t="s">
-        <v>134</v>
+        <v>133</v>
       </c>
       <c r="D34" t="s">
-        <v>136</v>
-      </c>
-    </row>
-    <row r="35" spans="1:4" x14ac:dyDescent="0.25">
+        <v>135</v>
+      </c>
+    </row>
+    <row r="35" spans="1:4">
       <c r="A35" t="s">
         <v>61</v>
       </c>
@@ -1331,13 +1336,13 @@
         <v>18</v>
       </c>
       <c r="C35" t="s">
-        <v>134</v>
+        <v>133</v>
       </c>
       <c r="D35" t="s">
-        <v>136</v>
-      </c>
-    </row>
-    <row r="36" spans="1:4" x14ac:dyDescent="0.25">
+        <v>135</v>
+      </c>
+    </row>
+    <row r="36" spans="1:4">
       <c r="A36" t="s">
         <v>85</v>
       </c>
@@ -1345,13 +1350,13 @@
         <v>3</v>
       </c>
       <c r="C36" t="s">
-        <v>134</v>
+        <v>133</v>
       </c>
       <c r="D36" t="s">
-        <v>136</v>
-      </c>
-    </row>
-    <row r="37" spans="1:4" x14ac:dyDescent="0.25">
+        <v>135</v>
+      </c>
+    </row>
+    <row r="37" spans="1:4">
       <c r="A37" t="s">
         <v>86</v>
       </c>
@@ -1359,13 +1364,13 @@
         <v>3</v>
       </c>
       <c r="C37" t="s">
-        <v>134</v>
+        <v>133</v>
       </c>
       <c r="D37" t="s">
-        <v>136</v>
-      </c>
-    </row>
-    <row r="38" spans="1:4" x14ac:dyDescent="0.25">
+        <v>135</v>
+      </c>
+    </row>
+    <row r="38" spans="1:4">
       <c r="A38" t="s">
         <v>62</v>
       </c>
@@ -1373,13 +1378,13 @@
         <v>3</v>
       </c>
       <c r="C38" t="s">
-        <v>134</v>
+        <v>133</v>
       </c>
       <c r="D38" t="s">
-        <v>136</v>
-      </c>
-    </row>
-    <row r="39" spans="1:4" x14ac:dyDescent="0.25">
+        <v>135</v>
+      </c>
+    </row>
+    <row r="39" spans="1:4">
       <c r="A39" t="s">
         <v>13</v>
       </c>
@@ -1387,13 +1392,13 @@
         <v>3</v>
       </c>
       <c r="C39" t="s">
+        <v>133</v>
+      </c>
+      <c r="D39" t="s">
         <v>134</v>
       </c>
-      <c r="D39" t="s">
-        <v>135</v>
-      </c>
-    </row>
-    <row r="40" spans="1:4" x14ac:dyDescent="0.25">
+    </row>
+    <row r="40" spans="1:4">
       <c r="A40" t="s">
         <v>37</v>
       </c>
@@ -1401,13 +1406,13 @@
         <v>3</v>
       </c>
       <c r="C40" t="s">
-        <v>134</v>
+        <v>133</v>
       </c>
       <c r="D40" t="s">
-        <v>136</v>
-      </c>
-    </row>
-    <row r="41" spans="1:4" x14ac:dyDescent="0.25">
+        <v>135</v>
+      </c>
+    </row>
+    <row r="41" spans="1:4">
       <c r="A41" t="s">
         <v>73</v>
       </c>
@@ -1415,13 +1420,13 @@
         <v>3</v>
       </c>
       <c r="C41" t="s">
-        <v>134</v>
+        <v>133</v>
       </c>
       <c r="D41" t="s">
-        <v>136</v>
-      </c>
-    </row>
-    <row r="42" spans="1:4" x14ac:dyDescent="0.25">
+        <v>135</v>
+      </c>
+    </row>
+    <row r="42" spans="1:4">
       <c r="A42" t="s">
         <v>28</v>
       </c>
@@ -1429,13 +1434,13 @@
         <v>18</v>
       </c>
       <c r="C42" t="s">
-        <v>134</v>
+        <v>133</v>
       </c>
       <c r="D42" t="s">
-        <v>136</v>
-      </c>
-    </row>
-    <row r="43" spans="1:4" x14ac:dyDescent="0.25">
+        <v>135</v>
+      </c>
+    </row>
+    <row r="43" spans="1:4">
       <c r="A43" t="s">
         <v>4</v>
       </c>
@@ -1443,13 +1448,13 @@
         <v>3</v>
       </c>
       <c r="C43" t="s">
+        <v>133</v>
+      </c>
+      <c r="D43" t="s">
         <v>134</v>
       </c>
-      <c r="D43" t="s">
-        <v>135</v>
-      </c>
-    </row>
-    <row r="44" spans="1:4" x14ac:dyDescent="0.25">
+    </row>
+    <row r="44" spans="1:4">
       <c r="A44" t="s">
         <v>126</v>
       </c>
@@ -1457,13 +1462,13 @@
         <v>3</v>
       </c>
       <c r="C44" t="s">
-        <v>134</v>
+        <v>133</v>
       </c>
       <c r="D44" t="s">
-        <v>136</v>
-      </c>
-    </row>
-    <row r="45" spans="1:4" x14ac:dyDescent="0.25">
+        <v>135</v>
+      </c>
+    </row>
+    <row r="45" spans="1:4">
       <c r="A45" t="s">
         <v>127</v>
       </c>
@@ -1471,13 +1476,13 @@
         <v>3</v>
       </c>
       <c r="C45" t="s">
-        <v>134</v>
+        <v>133</v>
       </c>
       <c r="D45" t="s">
-        <v>136</v>
-      </c>
-    </row>
-    <row r="46" spans="1:4" x14ac:dyDescent="0.25">
+        <v>135</v>
+      </c>
+    </row>
+    <row r="46" spans="1:4">
       <c r="A46" t="s">
         <v>128</v>
       </c>
@@ -1485,13 +1490,13 @@
         <v>3</v>
       </c>
       <c r="C46" t="s">
-        <v>134</v>
+        <v>133</v>
       </c>
       <c r="D46" t="s">
-        <v>136</v>
-      </c>
-    </row>
-    <row r="47" spans="1:4" x14ac:dyDescent="0.25">
+        <v>135</v>
+      </c>
+    </row>
+    <row r="47" spans="1:4">
       <c r="A47" t="s">
         <v>129</v>
       </c>
@@ -1499,13 +1504,13 @@
         <v>3</v>
       </c>
       <c r="C47" t="s">
-        <v>134</v>
+        <v>133</v>
       </c>
       <c r="D47" t="s">
-        <v>136</v>
-      </c>
-    </row>
-    <row r="48" spans="1:4" x14ac:dyDescent="0.25">
+        <v>135</v>
+      </c>
+    </row>
+    <row r="48" spans="1:4">
       <c r="A48" t="s">
         <v>87</v>
       </c>
@@ -1513,13 +1518,13 @@
         <v>3</v>
       </c>
       <c r="C48" t="s">
-        <v>134</v>
+        <v>133</v>
       </c>
       <c r="D48" t="s">
-        <v>136</v>
-      </c>
-    </row>
-    <row r="49" spans="1:4" x14ac:dyDescent="0.25">
+        <v>135</v>
+      </c>
+    </row>
+    <row r="49" spans="1:4">
       <c r="A49" t="s">
         <v>88</v>
       </c>
@@ -1527,13 +1532,13 @@
         <v>3</v>
       </c>
       <c r="C49" t="s">
-        <v>134</v>
+        <v>133</v>
       </c>
       <c r="D49" t="s">
-        <v>136</v>
-      </c>
-    </row>
-    <row r="50" spans="1:4" x14ac:dyDescent="0.25">
+        <v>135</v>
+      </c>
+    </row>
+    <row r="50" spans="1:4">
       <c r="A50" t="s">
         <v>89</v>
       </c>
@@ -1541,13 +1546,13 @@
         <v>3</v>
       </c>
       <c r="C50" t="s">
-        <v>134</v>
+        <v>133</v>
       </c>
       <c r="D50" t="s">
-        <v>136</v>
-      </c>
-    </row>
-    <row r="51" spans="1:4" x14ac:dyDescent="0.25">
+        <v>135</v>
+      </c>
+    </row>
+    <row r="51" spans="1:4">
       <c r="A51" t="s">
         <v>90</v>
       </c>
@@ -1555,13 +1560,13 @@
         <v>3</v>
       </c>
       <c r="C51" t="s">
-        <v>134</v>
+        <v>133</v>
       </c>
       <c r="D51" t="s">
-        <v>136</v>
-      </c>
-    </row>
-    <row r="52" spans="1:4" x14ac:dyDescent="0.25">
+        <v>135</v>
+      </c>
+    </row>
+    <row r="52" spans="1:4">
       <c r="A52" t="s">
         <v>91</v>
       </c>
@@ -1569,13 +1574,13 @@
         <v>3</v>
       </c>
       <c r="C52" t="s">
-        <v>134</v>
+        <v>133</v>
       </c>
       <c r="D52" t="s">
-        <v>136</v>
-      </c>
-    </row>
-    <row r="53" spans="1:4" x14ac:dyDescent="0.25">
+        <v>135</v>
+      </c>
+    </row>
+    <row r="53" spans="1:4">
       <c r="A53" t="s">
         <v>12</v>
       </c>
@@ -1583,13 +1588,13 @@
         <v>3</v>
       </c>
       <c r="C53" t="s">
-        <v>138</v>
+        <v>137</v>
       </c>
       <c r="D53" t="s">
-        <v>135</v>
-      </c>
-    </row>
-    <row r="54" spans="1:4" x14ac:dyDescent="0.25">
+        <v>134</v>
+      </c>
+    </row>
+    <row r="54" spans="1:4">
       <c r="A54" t="s">
         <v>11</v>
       </c>
@@ -1597,13 +1602,13 @@
         <v>3</v>
       </c>
       <c r="C54" t="s">
-        <v>138</v>
+        <v>137</v>
       </c>
       <c r="D54" t="s">
-        <v>135</v>
-      </c>
-    </row>
-    <row r="55" spans="1:4" x14ac:dyDescent="0.25">
+        <v>134</v>
+      </c>
+    </row>
+    <row r="55" spans="1:4">
       <c r="A55" t="s">
         <v>10</v>
       </c>
@@ -1611,13 +1616,13 @@
         <v>3</v>
       </c>
       <c r="C55" t="s">
-        <v>138</v>
+        <v>137</v>
       </c>
       <c r="D55" t="s">
-        <v>135</v>
-      </c>
-    </row>
-    <row r="56" spans="1:4" x14ac:dyDescent="0.25">
+        <v>134</v>
+      </c>
+    </row>
+    <row r="56" spans="1:4">
       <c r="A56" t="s">
         <v>40</v>
       </c>
@@ -1625,13 +1630,13 @@
         <v>3</v>
       </c>
       <c r="C56" t="s">
-        <v>138</v>
+        <v>137</v>
       </c>
       <c r="D56" t="s">
-        <v>135</v>
-      </c>
-    </row>
-    <row r="57" spans="1:4" x14ac:dyDescent="0.25">
+        <v>134</v>
+      </c>
+    </row>
+    <row r="57" spans="1:4">
       <c r="A57" t="s">
         <v>21</v>
       </c>
@@ -1639,13 +1644,13 @@
         <v>3</v>
       </c>
       <c r="C57" t="s">
-        <v>138</v>
+        <v>137</v>
       </c>
       <c r="D57" t="s">
-        <v>135</v>
-      </c>
-    </row>
-    <row r="58" spans="1:4" x14ac:dyDescent="0.25">
+        <v>134</v>
+      </c>
+    </row>
+    <row r="58" spans="1:4">
       <c r="A58" t="s">
         <v>70</v>
       </c>
@@ -1653,13 +1658,13 @@
         <v>3</v>
       </c>
       <c r="C58" t="s">
-        <v>134</v>
+        <v>133</v>
       </c>
       <c r="D58" t="s">
-        <v>136</v>
-      </c>
-    </row>
-    <row r="59" spans="1:4" x14ac:dyDescent="0.25">
+        <v>135</v>
+      </c>
+    </row>
+    <row r="59" spans="1:4">
       <c r="A59" t="s">
         <v>72</v>
       </c>
@@ -1667,13 +1672,13 @@
         <v>3</v>
       </c>
       <c r="C59" t="s">
-        <v>134</v>
+        <v>133</v>
       </c>
       <c r="D59" t="s">
-        <v>136</v>
-      </c>
-    </row>
-    <row r="60" spans="1:4" x14ac:dyDescent="0.25">
+        <v>135</v>
+      </c>
+    </row>
+    <row r="60" spans="1:4">
       <c r="A60" t="s">
         <v>104</v>
       </c>
@@ -1681,13 +1686,13 @@
         <v>3</v>
       </c>
       <c r="C60" t="s">
-        <v>134</v>
+        <v>133</v>
       </c>
       <c r="D60" t="s">
-        <v>136</v>
-      </c>
-    </row>
-    <row r="61" spans="1:4" x14ac:dyDescent="0.25">
+        <v>135</v>
+      </c>
+    </row>
+    <row r="61" spans="1:4">
       <c r="A61" t="s">
         <v>5</v>
       </c>
@@ -1695,13 +1700,13 @@
         <v>3</v>
       </c>
       <c r="C61" t="s">
-        <v>134</v>
+        <v>133</v>
       </c>
       <c r="D61" t="s">
-        <v>136</v>
-      </c>
-    </row>
-    <row r="62" spans="1:4" x14ac:dyDescent="0.25">
+        <v>135</v>
+      </c>
+    </row>
+    <row r="62" spans="1:4">
       <c r="A62" t="s">
         <v>116</v>
       </c>
@@ -1709,13 +1714,13 @@
         <v>3</v>
       </c>
       <c r="C62" t="s">
-        <v>134</v>
+        <v>133</v>
       </c>
       <c r="D62" t="s">
-        <v>136</v>
-      </c>
-    </row>
-    <row r="63" spans="1:4" x14ac:dyDescent="0.25">
+        <v>135</v>
+      </c>
+    </row>
+    <row r="63" spans="1:4">
       <c r="A63" t="s">
         <v>92</v>
       </c>
@@ -1723,13 +1728,13 @@
         <v>3</v>
       </c>
       <c r="C63" t="s">
-        <v>134</v>
+        <v>133</v>
       </c>
       <c r="D63" t="s">
-        <v>136</v>
-      </c>
-    </row>
-    <row r="64" spans="1:4" x14ac:dyDescent="0.25">
+        <v>135</v>
+      </c>
+    </row>
+    <row r="64" spans="1:4">
       <c r="A64" t="s">
         <v>130</v>
       </c>
@@ -1737,13 +1742,13 @@
         <v>3</v>
       </c>
       <c r="C64" t="s">
-        <v>134</v>
+        <v>133</v>
       </c>
       <c r="D64" t="s">
-        <v>136</v>
-      </c>
-    </row>
-    <row r="65" spans="1:4" x14ac:dyDescent="0.25">
+        <v>135</v>
+      </c>
+    </row>
+    <row r="65" spans="1:4">
       <c r="A65" t="s">
         <v>16</v>
       </c>
@@ -1751,13 +1756,13 @@
         <v>3</v>
       </c>
       <c r="C65" t="s">
-        <v>134</v>
+        <v>133</v>
       </c>
       <c r="D65" t="s">
-        <v>136</v>
-      </c>
-    </row>
-    <row r="66" spans="1:4" x14ac:dyDescent="0.25">
+        <v>135</v>
+      </c>
+    </row>
+    <row r="66" spans="1:4">
       <c r="A66" t="s">
         <v>63</v>
       </c>
@@ -1765,13 +1770,13 @@
         <v>18</v>
       </c>
       <c r="C66" t="s">
-        <v>134</v>
+        <v>133</v>
       </c>
       <c r="D66" t="s">
-        <v>136</v>
-      </c>
-    </row>
-    <row r="67" spans="1:4" x14ac:dyDescent="0.25">
+        <v>135</v>
+      </c>
+    </row>
+    <row r="67" spans="1:4">
       <c r="A67" t="s">
         <v>112</v>
       </c>
@@ -1779,13 +1784,13 @@
         <v>3</v>
       </c>
       <c r="C67" t="s">
-        <v>134</v>
+        <v>133</v>
       </c>
       <c r="D67" t="s">
-        <v>136</v>
-      </c>
-    </row>
-    <row r="68" spans="1:4" x14ac:dyDescent="0.25">
+        <v>135</v>
+      </c>
+    </row>
+    <row r="68" spans="1:4">
       <c r="A68" t="s">
         <v>6</v>
       </c>
@@ -1793,13 +1798,13 @@
         <v>3</v>
       </c>
       <c r="C68" t="s">
-        <v>137</v>
+        <v>136</v>
       </c>
       <c r="D68" t="s">
-        <v>135</v>
-      </c>
-    </row>
-    <row r="69" spans="1:4" x14ac:dyDescent="0.25">
+        <v>134</v>
+      </c>
+    </row>
+    <row r="69" spans="1:4">
       <c r="A69" t="s">
         <v>44</v>
       </c>
@@ -1807,13 +1812,13 @@
         <v>3</v>
       </c>
       <c r="C69" t="s">
-        <v>134</v>
+        <v>133</v>
       </c>
       <c r="D69" t="s">
-        <v>136</v>
-      </c>
-    </row>
-    <row r="70" spans="1:4" x14ac:dyDescent="0.25">
+        <v>135</v>
+      </c>
+    </row>
+    <row r="70" spans="1:4">
       <c r="A70" t="s">
         <v>56</v>
       </c>
@@ -1821,13 +1826,13 @@
         <v>3</v>
       </c>
       <c r="C70" t="s">
-        <v>134</v>
+        <v>133</v>
       </c>
       <c r="D70" t="s">
-        <v>136</v>
-      </c>
-    </row>
-    <row r="71" spans="1:4" x14ac:dyDescent="0.25">
+        <v>135</v>
+      </c>
+    </row>
+    <row r="71" spans="1:4">
       <c r="A71" t="s">
         <v>45</v>
       </c>
@@ -1835,13 +1840,13 @@
         <v>3</v>
       </c>
       <c r="C71" t="s">
-        <v>134</v>
+        <v>133</v>
       </c>
       <c r="D71" t="s">
-        <v>136</v>
-      </c>
-    </row>
-    <row r="72" spans="1:4" x14ac:dyDescent="0.25">
+        <v>135</v>
+      </c>
+    </row>
+    <row r="72" spans="1:4">
       <c r="A72" t="s">
         <v>46</v>
       </c>
@@ -1849,13 +1854,13 @@
         <v>3</v>
       </c>
       <c r="C72" t="s">
-        <v>134</v>
+        <v>133</v>
       </c>
       <c r="D72" t="s">
-        <v>136</v>
-      </c>
-    </row>
-    <row r="73" spans="1:4" x14ac:dyDescent="0.25">
+        <v>135</v>
+      </c>
+    </row>
+    <row r="73" spans="1:4">
       <c r="A73" t="s">
         <v>47</v>
       </c>
@@ -1863,13 +1868,13 @@
         <v>3</v>
       </c>
       <c r="C73" t="s">
-        <v>134</v>
+        <v>133</v>
       </c>
       <c r="D73" t="s">
-        <v>136</v>
-      </c>
-    </row>
-    <row r="74" spans="1:4" x14ac:dyDescent="0.25">
+        <v>135</v>
+      </c>
+    </row>
+    <row r="74" spans="1:4">
       <c r="A74" t="s">
         <v>7</v>
       </c>
@@ -1877,13 +1882,13 @@
         <v>3</v>
       </c>
       <c r="C74" t="s">
+        <v>133</v>
+      </c>
+      <c r="D74" t="s">
         <v>134</v>
       </c>
-      <c r="D74" t="s">
-        <v>135</v>
-      </c>
-    </row>
-    <row r="75" spans="1:4" x14ac:dyDescent="0.25">
+    </row>
+    <row r="75" spans="1:4">
       <c r="A75" t="s">
         <v>64</v>
       </c>
@@ -1891,13 +1896,13 @@
         <v>3</v>
       </c>
       <c r="C75" t="s">
-        <v>134</v>
+        <v>133</v>
       </c>
       <c r="D75" t="s">
-        <v>136</v>
-      </c>
-    </row>
-    <row r="76" spans="1:4" x14ac:dyDescent="0.25">
+        <v>135</v>
+      </c>
+    </row>
+    <row r="76" spans="1:4">
       <c r="A76" t="s">
         <v>96</v>
       </c>
@@ -1905,13 +1910,13 @@
         <v>3</v>
       </c>
       <c r="C76" t="s">
-        <v>134</v>
+        <v>133</v>
       </c>
       <c r="D76" t="s">
-        <v>136</v>
-      </c>
-    </row>
-    <row r="77" spans="1:4" x14ac:dyDescent="0.25">
+        <v>135</v>
+      </c>
+    </row>
+    <row r="77" spans="1:4">
       <c r="A77" t="s">
         <v>97</v>
       </c>
@@ -1919,13 +1924,13 @@
         <v>18</v>
       </c>
       <c r="C77" t="s">
-        <v>134</v>
+        <v>133</v>
       </c>
       <c r="D77" t="s">
-        <v>136</v>
-      </c>
-    </row>
-    <row r="78" spans="1:4" x14ac:dyDescent="0.25">
+        <v>135</v>
+      </c>
+    </row>
+    <row r="78" spans="1:4">
       <c r="A78" t="s">
         <v>105</v>
       </c>
@@ -1933,13 +1938,13 @@
         <v>18</v>
       </c>
       <c r="C78" t="s">
-        <v>134</v>
+        <v>133</v>
       </c>
       <c r="D78" t="s">
-        <v>136</v>
-      </c>
-    </row>
-    <row r="79" spans="1:4" x14ac:dyDescent="0.25">
+        <v>135</v>
+      </c>
+    </row>
+    <row r="79" spans="1:4">
       <c r="A79" t="s">
         <v>23</v>
       </c>
@@ -1947,13 +1952,13 @@
         <v>18</v>
       </c>
       <c r="C79" t="s">
-        <v>134</v>
+        <v>133</v>
       </c>
       <c r="D79" t="s">
-        <v>136</v>
-      </c>
-    </row>
-    <row r="80" spans="1:4" x14ac:dyDescent="0.25">
+        <v>135</v>
+      </c>
+    </row>
+    <row r="80" spans="1:4">
       <c r="A80" t="s">
         <v>79</v>
       </c>
@@ -1961,13 +1966,13 @@
         <v>18</v>
       </c>
       <c r="C80" t="s">
-        <v>134</v>
+        <v>133</v>
       </c>
       <c r="D80" t="s">
-        <v>136</v>
-      </c>
-    </row>
-    <row r="81" spans="1:4" x14ac:dyDescent="0.25">
+        <v>135</v>
+      </c>
+    </row>
+    <row r="81" spans="1:4">
       <c r="A81" t="s">
         <v>65</v>
       </c>
@@ -1975,13 +1980,13 @@
         <v>18</v>
       </c>
       <c r="C81" t="s">
-        <v>134</v>
+        <v>133</v>
       </c>
       <c r="D81" t="s">
-        <v>136</v>
-      </c>
-    </row>
-    <row r="82" spans="1:4" x14ac:dyDescent="0.25">
+        <v>135</v>
+      </c>
+    </row>
+    <row r="82" spans="1:4">
       <c r="A82" t="s">
         <v>98</v>
       </c>
@@ -1989,13 +1994,13 @@
         <v>18</v>
       </c>
       <c r="C82" t="s">
-        <v>134</v>
+        <v>133</v>
       </c>
       <c r="D82" t="s">
-        <v>136</v>
-      </c>
-    </row>
-    <row r="83" spans="1:4" x14ac:dyDescent="0.25">
+        <v>135</v>
+      </c>
+    </row>
+    <row r="83" spans="1:4">
       <c r="A83" t="s">
         <v>66</v>
       </c>
@@ -2003,13 +2008,13 @@
         <v>18</v>
       </c>
       <c r="C83" t="s">
-        <v>134</v>
+        <v>133</v>
       </c>
       <c r="D83" t="s">
-        <v>136</v>
-      </c>
-    </row>
-    <row r="84" spans="1:4" x14ac:dyDescent="0.25">
+        <v>135</v>
+      </c>
+    </row>
+    <row r="84" spans="1:4">
       <c r="A84" t="s">
         <v>106</v>
       </c>
@@ -2017,13 +2022,13 @@
         <v>18</v>
       </c>
       <c r="C84" t="s">
-        <v>134</v>
+        <v>133</v>
       </c>
       <c r="D84" t="s">
-        <v>136</v>
-      </c>
-    </row>
-    <row r="85" spans="1:4" x14ac:dyDescent="0.25">
+        <v>135</v>
+      </c>
+    </row>
+    <row r="85" spans="1:4">
       <c r="A85" t="s">
         <v>107</v>
       </c>
@@ -2031,13 +2036,13 @@
         <v>18</v>
       </c>
       <c r="C85" t="s">
-        <v>134</v>
+        <v>133</v>
       </c>
       <c r="D85" t="s">
-        <v>136</v>
-      </c>
-    </row>
-    <row r="86" spans="1:4" x14ac:dyDescent="0.25">
+        <v>135</v>
+      </c>
+    </row>
+    <row r="86" spans="1:4">
       <c r="A86" t="s">
         <v>110</v>
       </c>
@@ -2045,13 +2050,13 @@
         <v>18</v>
       </c>
       <c r="C86" t="s">
-        <v>134</v>
+        <v>133</v>
       </c>
       <c r="D86" t="s">
-        <v>136</v>
-      </c>
-    </row>
-    <row r="87" spans="1:4" x14ac:dyDescent="0.25">
+        <v>135</v>
+      </c>
+    </row>
+    <row r="87" spans="1:4">
       <c r="A87" t="s">
         <v>8</v>
       </c>
@@ -2059,13 +2064,13 @@
         <v>3</v>
       </c>
       <c r="C87" t="s">
+        <v>133</v>
+      </c>
+      <c r="D87" t="s">
         <v>134</v>
       </c>
-      <c r="D87" t="s">
-        <v>135</v>
-      </c>
-    </row>
-    <row r="88" spans="1:4" x14ac:dyDescent="0.25">
+    </row>
+    <row r="88" spans="1:4">
       <c r="A88" t="s">
         <v>48</v>
       </c>
@@ -2073,13 +2078,13 @@
         <v>3</v>
       </c>
       <c r="C88" t="s">
-        <v>134</v>
+        <v>133</v>
       </c>
       <c r="D88" t="s">
-        <v>136</v>
-      </c>
-    </row>
-    <row r="89" spans="1:4" x14ac:dyDescent="0.25">
+        <v>135</v>
+      </c>
+    </row>
+    <row r="89" spans="1:4">
       <c r="A89" t="s">
         <v>26</v>
       </c>
@@ -2087,13 +2092,13 @@
         <v>18</v>
       </c>
       <c r="C89" t="s">
-        <v>134</v>
+        <v>133</v>
       </c>
       <c r="D89" t="s">
-        <v>136</v>
-      </c>
-    </row>
-    <row r="90" spans="1:4" x14ac:dyDescent="0.25">
+        <v>135</v>
+      </c>
+    </row>
+    <row r="90" spans="1:4">
       <c r="A90" t="s">
         <v>49</v>
       </c>
@@ -2101,13 +2106,13 @@
         <v>3</v>
       </c>
       <c r="C90" t="s">
-        <v>134</v>
+        <v>133</v>
       </c>
       <c r="D90" t="s">
-        <v>136</v>
-      </c>
-    </row>
-    <row r="91" spans="1:4" x14ac:dyDescent="0.25">
+        <v>135</v>
+      </c>
+    </row>
+    <row r="91" spans="1:4">
       <c r="A91" t="s">
         <v>99</v>
       </c>
@@ -2115,13 +2120,13 @@
         <v>18</v>
       </c>
       <c r="C91" t="s">
-        <v>134</v>
+        <v>133</v>
       </c>
       <c r="D91" t="s">
-        <v>136</v>
-      </c>
-    </row>
-    <row r="92" spans="1:4" x14ac:dyDescent="0.25">
+        <v>135</v>
+      </c>
+    </row>
+    <row r="92" spans="1:4">
       <c r="A92" t="s">
         <v>67</v>
       </c>
@@ -2129,13 +2134,13 @@
         <v>18</v>
       </c>
       <c r="C92" t="s">
-        <v>134</v>
+        <v>133</v>
       </c>
       <c r="D92" t="s">
-        <v>136</v>
-      </c>
-    </row>
-    <row r="93" spans="1:4" x14ac:dyDescent="0.25">
+        <v>135</v>
+      </c>
+    </row>
+    <row r="93" spans="1:4">
       <c r="A93" t="s">
         <v>19</v>
       </c>
@@ -2143,13 +2148,13 @@
         <v>3</v>
       </c>
       <c r="C93" t="s">
-        <v>134</v>
+        <v>133</v>
       </c>
       <c r="D93" t="s">
-        <v>136</v>
-      </c>
-    </row>
-    <row r="94" spans="1:4" x14ac:dyDescent="0.25">
+        <v>135</v>
+      </c>
+    </row>
+    <row r="94" spans="1:4">
       <c r="A94" t="s">
         <v>119</v>
       </c>
@@ -2157,13 +2162,13 @@
         <v>3</v>
       </c>
       <c r="C94" t="s">
-        <v>134</v>
+        <v>133</v>
       </c>
       <c r="D94" t="s">
-        <v>136</v>
-      </c>
-    </row>
-    <row r="95" spans="1:4" x14ac:dyDescent="0.25">
+        <v>135</v>
+      </c>
+    </row>
+    <row r="95" spans="1:4">
       <c r="A95" t="s">
         <v>24</v>
       </c>
@@ -2171,13 +2176,13 @@
         <v>3</v>
       </c>
       <c r="C95" t="s">
-        <v>134</v>
+        <v>133</v>
       </c>
       <c r="D95" t="s">
-        <v>136</v>
-      </c>
-    </row>
-    <row r="96" spans="1:4" x14ac:dyDescent="0.25">
+        <v>135</v>
+      </c>
+    </row>
+    <row r="96" spans="1:4">
       <c r="A96" t="s">
         <v>57</v>
       </c>
@@ -2185,13 +2190,13 @@
         <v>3</v>
       </c>
       <c r="C96" t="s">
-        <v>134</v>
+        <v>133</v>
       </c>
       <c r="D96" t="s">
-        <v>136</v>
-      </c>
-    </row>
-    <row r="97" spans="1:4" x14ac:dyDescent="0.25">
+        <v>135</v>
+      </c>
+    </row>
+    <row r="97" spans="1:4">
       <c r="A97" t="s">
         <v>50</v>
       </c>
@@ -2199,13 +2204,13 @@
         <v>3</v>
       </c>
       <c r="C97" t="s">
-        <v>134</v>
+        <v>133</v>
       </c>
       <c r="D97" t="s">
-        <v>136</v>
-      </c>
-    </row>
-    <row r="98" spans="1:4" x14ac:dyDescent="0.25">
+        <v>135</v>
+      </c>
+    </row>
+    <row r="98" spans="1:4">
       <c r="A98" t="s">
         <v>25</v>
       </c>
@@ -2213,13 +2218,13 @@
         <v>3</v>
       </c>
       <c r="C98" t="s">
-        <v>134</v>
+        <v>133</v>
       </c>
       <c r="D98" t="s">
-        <v>136</v>
-      </c>
-    </row>
-    <row r="99" spans="1:4" x14ac:dyDescent="0.25">
+        <v>135</v>
+      </c>
+    </row>
+    <row r="99" spans="1:4">
       <c r="A99" t="s">
         <v>9</v>
       </c>
@@ -2227,13 +2232,13 @@
         <v>3</v>
       </c>
       <c r="C99" t="s">
+        <v>133</v>
+      </c>
+      <c r="D99" t="s">
         <v>134</v>
       </c>
-      <c r="D99" t="s">
-        <v>135</v>
-      </c>
-    </row>
-    <row r="100" spans="1:4" x14ac:dyDescent="0.25">
+    </row>
+    <row r="100" spans="1:4">
       <c r="A100" t="s">
         <v>2</v>
       </c>
@@ -2241,13 +2246,13 @@
         <v>3</v>
       </c>
       <c r="C100" t="s">
+        <v>133</v>
+      </c>
+      <c r="D100" t="s">
         <v>134</v>
       </c>
-      <c r="D100" t="s">
-        <v>135</v>
-      </c>
-    </row>
-    <row r="101" spans="1:4" x14ac:dyDescent="0.25">
+    </row>
+    <row r="101" spans="1:4">
       <c r="A101" t="s">
         <v>122</v>
       </c>
@@ -2255,13 +2260,13 @@
         <v>3</v>
       </c>
       <c r="C101" t="s">
-        <v>134</v>
+        <v>133</v>
       </c>
       <c r="D101" t="s">
-        <v>136</v>
-      </c>
-    </row>
-    <row r="102" spans="1:4" x14ac:dyDescent="0.25">
+        <v>135</v>
+      </c>
+    </row>
+    <row r="102" spans="1:4">
       <c r="A102" t="s">
         <v>32</v>
       </c>
@@ -2269,13 +2274,13 @@
         <v>18</v>
       </c>
       <c r="C102" t="s">
-        <v>134</v>
+        <v>133</v>
       </c>
       <c r="D102" t="s">
-        <v>136</v>
-      </c>
-    </row>
-    <row r="103" spans="1:4" x14ac:dyDescent="0.25">
+        <v>135</v>
+      </c>
+    </row>
+    <row r="103" spans="1:4">
       <c r="A103" t="s">
         <v>75</v>
       </c>
@@ -2283,13 +2288,13 @@
         <v>18</v>
       </c>
       <c r="C103" t="s">
-        <v>134</v>
+        <v>133</v>
       </c>
       <c r="D103" t="s">
-        <v>136</v>
-      </c>
-    </row>
-    <row r="104" spans="1:4" x14ac:dyDescent="0.25">
+        <v>135</v>
+      </c>
+    </row>
+    <row r="104" spans="1:4">
       <c r="A104" t="s">
         <v>114</v>
       </c>
@@ -2297,13 +2302,13 @@
         <v>18</v>
       </c>
       <c r="C104" t="s">
-        <v>134</v>
+        <v>133</v>
       </c>
       <c r="D104" t="s">
-        <v>136</v>
-      </c>
-    </row>
-    <row r="105" spans="1:4" x14ac:dyDescent="0.25">
+        <v>135</v>
+      </c>
+    </row>
+    <row r="105" spans="1:4">
       <c r="A105" t="s">
         <v>17</v>
       </c>
@@ -2311,13 +2316,13 @@
         <v>18</v>
       </c>
       <c r="C105" t="s">
-        <v>134</v>
+        <v>133</v>
       </c>
       <c r="D105" t="s">
-        <v>136</v>
-      </c>
-    </row>
-    <row r="106" spans="1:4" x14ac:dyDescent="0.25">
+        <v>135</v>
+      </c>
+    </row>
+    <row r="106" spans="1:4">
       <c r="A106" t="s">
         <v>115</v>
       </c>
@@ -2325,13 +2330,13 @@
         <v>18</v>
       </c>
       <c r="C106" t="s">
-        <v>134</v>
+        <v>133</v>
       </c>
       <c r="D106" t="s">
-        <v>136</v>
-      </c>
-    </row>
-    <row r="107" spans="1:4" x14ac:dyDescent="0.25">
+        <v>135</v>
+      </c>
+    </row>
+    <row r="107" spans="1:4">
       <c r="A107" t="s">
         <v>125</v>
       </c>
@@ -2339,13 +2344,13 @@
         <v>18</v>
       </c>
       <c r="C107" t="s">
-        <v>134</v>
+        <v>133</v>
       </c>
       <c r="D107" t="s">
-        <v>136</v>
-      </c>
-    </row>
-    <row r="108" spans="1:4" x14ac:dyDescent="0.25">
+        <v>135</v>
+      </c>
+    </row>
+    <row r="108" spans="1:4">
       <c r="A108" t="s">
         <v>108</v>
       </c>
@@ -2353,13 +2358,13 @@
         <v>18</v>
       </c>
       <c r="C108" t="s">
-        <v>134</v>
+        <v>133</v>
       </c>
       <c r="D108" t="s">
-        <v>136</v>
-      </c>
-    </row>
-    <row r="109" spans="1:4" x14ac:dyDescent="0.25">
+        <v>135</v>
+      </c>
+    </row>
+    <row r="109" spans="1:4">
       <c r="A109" t="s">
         <v>109</v>
       </c>
@@ -2367,13 +2372,13 @@
         <v>18</v>
       </c>
       <c r="C109" t="s">
-        <v>134</v>
+        <v>133</v>
       </c>
       <c r="D109" t="s">
-        <v>136</v>
-      </c>
-    </row>
-    <row r="110" spans="1:4" x14ac:dyDescent="0.25">
+        <v>135</v>
+      </c>
+    </row>
+    <row r="110" spans="1:4">
       <c r="A110" t="s">
         <v>20</v>
       </c>
@@ -2381,13 +2386,13 @@
         <v>3</v>
       </c>
       <c r="C110" t="s">
-        <v>134</v>
+        <v>133</v>
       </c>
       <c r="D110" t="s">
-        <v>136</v>
-      </c>
-    </row>
-    <row r="111" spans="1:4" x14ac:dyDescent="0.25">
+        <v>135</v>
+      </c>
+    </row>
+    <row r="111" spans="1:4">
       <c r="A111" t="s">
         <v>111</v>
       </c>
@@ -2395,13 +2400,13 @@
         <v>3</v>
       </c>
       <c r="C111" t="s">
-        <v>134</v>
+        <v>133</v>
       </c>
       <c r="D111" t="s">
-        <v>136</v>
-      </c>
-    </row>
-    <row r="112" spans="1:4" x14ac:dyDescent="0.25">
+        <v>135</v>
+      </c>
+    </row>
+    <row r="112" spans="1:4">
       <c r="A112" t="s">
         <v>38</v>
       </c>
@@ -2409,13 +2414,13 @@
         <v>3</v>
       </c>
       <c r="C112" t="s">
+        <v>133</v>
+      </c>
+      <c r="D112" t="s">
         <v>134</v>
       </c>
-      <c r="D112" t="s">
-        <v>135</v>
-      </c>
-    </row>
-    <row r="113" spans="1:4" x14ac:dyDescent="0.25">
+    </row>
+    <row r="113" spans="1:4">
       <c r="A113" t="s">
         <v>39</v>
       </c>
@@ -2423,13 +2428,13 @@
         <v>3</v>
       </c>
       <c r="C113" t="s">
-        <v>134</v>
+        <v>133</v>
       </c>
       <c r="D113" t="s">
-        <v>136</v>
-      </c>
-    </row>
-    <row r="114" spans="1:4" x14ac:dyDescent="0.25">
+        <v>135</v>
+      </c>
+    </row>
+    <row r="114" spans="1:4">
       <c r="A114" t="s">
         <v>121</v>
       </c>
@@ -2437,13 +2442,13 @@
         <v>3</v>
       </c>
       <c r="C114" t="s">
-        <v>134</v>
+        <v>133</v>
       </c>
       <c r="D114" t="s">
-        <v>136</v>
-      </c>
-    </row>
-    <row r="115" spans="1:4" x14ac:dyDescent="0.25">
+        <v>135</v>
+      </c>
+    </row>
+    <row r="115" spans="1:4">
       <c r="A115" t="s">
         <v>76</v>
       </c>
@@ -2451,13 +2456,13 @@
         <v>18</v>
       </c>
       <c r="C115" t="s">
-        <v>134</v>
+        <v>133</v>
       </c>
       <c r="D115" t="s">
-        <v>136</v>
-      </c>
-    </row>
-    <row r="116" spans="1:4" x14ac:dyDescent="0.25">
+        <v>135</v>
+      </c>
+    </row>
+    <row r="116" spans="1:4">
       <c r="A116" t="s">
         <v>131</v>
       </c>
@@ -2465,13 +2470,13 @@
         <v>3</v>
       </c>
       <c r="C116" t="s">
-        <v>134</v>
+        <v>133</v>
       </c>
       <c r="D116" t="s">
-        <v>136</v>
-      </c>
-    </row>
-    <row r="117" spans="1:4" x14ac:dyDescent="0.25">
+        <v>135</v>
+      </c>
+    </row>
+    <row r="117" spans="1:4">
       <c r="A117" t="s">
         <v>113</v>
       </c>
@@ -2479,13 +2484,13 @@
         <v>3</v>
       </c>
       <c r="C117" t="s">
-        <v>134</v>
+        <v>133</v>
       </c>
       <c r="D117" t="s">
-        <v>136</v>
-      </c>
-    </row>
-    <row r="118" spans="1:4" x14ac:dyDescent="0.25">
+        <v>135</v>
+      </c>
+    </row>
+    <row r="118" spans="1:4">
       <c r="A118" t="s">
         <v>74</v>
       </c>
@@ -2493,13 +2498,13 @@
         <v>18</v>
       </c>
       <c r="C118" t="s">
-        <v>134</v>
+        <v>133</v>
       </c>
       <c r="D118" t="s">
-        <v>136</v>
-      </c>
-    </row>
-    <row r="119" spans="1:4" x14ac:dyDescent="0.25">
+        <v>135</v>
+      </c>
+    </row>
+    <row r="119" spans="1:4">
       <c r="A119" t="s">
         <v>41</v>
       </c>
@@ -2507,13 +2512,13 @@
         <v>18</v>
       </c>
       <c r="C119" t="s">
-        <v>134</v>
+        <v>133</v>
       </c>
       <c r="D119" t="s">
-        <v>136</v>
-      </c>
-    </row>
-    <row r="120" spans="1:4" x14ac:dyDescent="0.25">
+        <v>135</v>
+      </c>
+    </row>
+    <row r="120" spans="1:4">
       <c r="A120" t="s">
         <v>77</v>
       </c>
@@ -2521,13 +2526,13 @@
         <v>18</v>
       </c>
       <c r="C120" t="s">
-        <v>134</v>
+        <v>133</v>
       </c>
       <c r="D120" t="s">
-        <v>136</v>
-      </c>
-    </row>
-    <row r="121" spans="1:4" x14ac:dyDescent="0.25">
+        <v>135</v>
+      </c>
+    </row>
+    <row r="121" spans="1:4">
       <c r="A121" t="s">
         <v>51</v>
       </c>
@@ -2535,13 +2540,13 @@
         <v>18</v>
       </c>
       <c r="C121" t="s">
-        <v>134</v>
+        <v>133</v>
       </c>
       <c r="D121" t="s">
-        <v>136</v>
-      </c>
-    </row>
-    <row r="122" spans="1:4" x14ac:dyDescent="0.25">
+        <v>135</v>
+      </c>
+    </row>
+    <row r="122" spans="1:4">
       <c r="A122" t="s">
         <v>68</v>
       </c>
@@ -2549,13 +2554,13 @@
         <v>18</v>
       </c>
       <c r="C122" t="s">
-        <v>134</v>
+        <v>133</v>
       </c>
       <c r="D122" t="s">
-        <v>136</v>
-      </c>
-    </row>
-    <row r="123" spans="1:4" x14ac:dyDescent="0.25">
+        <v>135</v>
+      </c>
+    </row>
+    <row r="123" spans="1:4">
       <c r="A123" t="s">
         <v>69</v>
       </c>
@@ -2563,13 +2568,13 @@
         <v>18</v>
       </c>
       <c r="C123" t="s">
-        <v>134</v>
+        <v>133</v>
       </c>
       <c r="D123" t="s">
-        <v>136</v>
-      </c>
-    </row>
-    <row r="124" spans="1:4" x14ac:dyDescent="0.25">
+        <v>135</v>
+      </c>
+    </row>
+    <row r="124" spans="1:4">
       <c r="A124" t="s">
         <v>30</v>
       </c>
@@ -2577,13 +2582,13 @@
         <v>18</v>
       </c>
       <c r="C124" t="s">
-        <v>134</v>
+        <v>133</v>
       </c>
       <c r="D124" t="s">
-        <v>136</v>
-      </c>
-    </row>
-    <row r="125" spans="1:4" x14ac:dyDescent="0.25">
+        <v>135</v>
+      </c>
+    </row>
+    <row r="125" spans="1:4">
       <c r="A125" t="s">
         <v>52</v>
       </c>
@@ -2591,13 +2596,13 @@
         <v>18</v>
       </c>
       <c r="C125" t="s">
-        <v>134</v>
+        <v>133</v>
       </c>
       <c r="D125" t="s">
-        <v>136</v>
-      </c>
-    </row>
-    <row r="126" spans="1:4" x14ac:dyDescent="0.25">
+        <v>135</v>
+      </c>
+    </row>
+    <row r="126" spans="1:4">
       <c r="A126" t="s">
         <v>53</v>
       </c>
@@ -2605,13 +2610,13 @@
         <v>18</v>
       </c>
       <c r="C126" t="s">
-        <v>134</v>
+        <v>133</v>
       </c>
       <c r="D126" t="s">
-        <v>136</v>
-      </c>
-    </row>
-    <row r="127" spans="1:4" x14ac:dyDescent="0.25">
+        <v>135</v>
+      </c>
+    </row>
+    <row r="127" spans="1:4">
       <c r="A127" t="s">
         <v>100</v>
       </c>
@@ -2619,13 +2624,13 @@
         <v>18</v>
       </c>
       <c r="C127" t="s">
-        <v>134</v>
+        <v>133</v>
       </c>
       <c r="D127" t="s">
-        <v>136</v>
-      </c>
-    </row>
-    <row r="128" spans="1:4" x14ac:dyDescent="0.25">
+        <v>135</v>
+      </c>
+    </row>
+    <row r="128" spans="1:4">
       <c r="A128" t="s">
         <v>101</v>
       </c>
@@ -2633,13 +2638,13 @@
         <v>18</v>
       </c>
       <c r="C128" t="s">
-        <v>134</v>
+        <v>133</v>
       </c>
       <c r="D128" t="s">
-        <v>136</v>
-      </c>
-    </row>
-    <row r="129" spans="1:4" x14ac:dyDescent="0.25">
+        <v>135</v>
+      </c>
+    </row>
+    <row r="129" spans="1:4">
       <c r="A129" t="s">
         <v>54</v>
       </c>
@@ -2647,10 +2652,10 @@
         <v>18</v>
       </c>
       <c r="C129" t="s">
-        <v>134</v>
+        <v>133</v>
       </c>
       <c r="D129" t="s">
-        <v>136</v>
+        <v>135</v>
       </c>
     </row>
   </sheetData>
@@ -2660,7 +2665,12 @@
     </sortState>
   </autoFilter>
   <pageMargins left="0.511811024" right="0.511811024" top="0.78740157499999996" bottom="0.78740157499999996" header="0.31496062000000002" footer="0.31496062000000002"/>
-  <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
+  <pageSetup paperSize="9" orientation="portrait"/>
+  <extLst>
+    <ext xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" uri="{64002731-A6B0-56B0-2670-7721B7C09600}">
+      <mx:PLV Mode="0" OnePage="0" WScale="0"/>
+    </ext>
+  </extLst>
 </worksheet>
 </file>
 
@@ -2670,9 +2680,14 @@
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="14" x14ac:dyDescent="0"/>
   <sheetData/>
   <pageMargins left="0.511811024" right="0.511811024" top="0.78740157499999996" bottom="0.78740157499999996" header="0.31496062000000002" footer="0.31496062000000002"/>
+  <extLst>
+    <ext xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" uri="{64002731-A6B0-56B0-2670-7721B7C09600}">
+      <mx:PLV Mode="0" OnePage="0" WScale="0"/>
+    </ext>
+  </extLst>
 </worksheet>
 </file>
 
@@ -2682,8 +2697,13 @@
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="14" x14ac:dyDescent="0"/>
   <sheetData/>
   <pageMargins left="0.511811024" right="0.511811024" top="0.78740157499999996" bottom="0.78740157499999996" header="0.31496062000000002" footer="0.31496062000000002"/>
+  <extLst>
+    <ext xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" uri="{64002731-A6B0-56B0-2670-7721B7C09600}">
+      <mx:PLV Mode="0" OnePage="0" WScale="0"/>
+    </ext>
+  </extLst>
 </worksheet>
 </file>
</xml_diff>